<commit_message>
.TEX: worked on Intro
</commit_message>
<xml_diff>
--- a/FORTRAN_code/TEST_11062015.xlsx
+++ b/FORTRAN_code/TEST_11062015.xlsx
@@ -279,10 +279,10 @@
     <t>TEST 11</t>
   </si>
   <si>
-    <t>U(n,n) small   9.50561683795606015E-033</t>
-  </si>
-  <si>
-    <t>33          26</t>
+    <t>loc_k = 3</t>
+  </si>
+  <si>
+    <t>           33          26</t>
   </si>
   <si>
     <t>Warning: Matrix is close to singular or badly scaled. Results may be inaccurate. RCOND =  2.346852e-45.</t>
@@ -2046,6 +2046,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2063,10 +2067,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2201,8 +2201,8 @@
   </sheetPr>
   <dimension ref="A5:J211"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B177" activeCellId="0" sqref="B177"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4350,74 +4350,76 @@
         <v>2</v>
       </c>
     </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>1677.88</v>
       </c>
-      <c r="D180" s="0" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B181" s="0" t="s">
         <v>87</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="E181" s="0" t="n">
-        <v>0.32467345388171</v>
+        <v>0.298996746825692</v>
       </c>
       <c r="G181" s="0" t="n">
-        <v>0.3247</v>
+        <v>0.299</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>6.9125409346496</v>
+        <v>6.91253698677764</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="E182" s="6" t="n">
-        <v>-4.67208357603601E-005</v>
+        <v>-4.57004616227985E-005</v>
       </c>
       <c r="G182" s="6" t="n">
-        <v>-4.6719E-005</v>
+        <v>-4.5699E-005</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B183" s="6" t="n">
-        <v>0.00143542327158778</v>
+        <v>0.00143656995180463</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="E183" s="0" t="n">
-        <v>0.32467345388171</v>
+        <v>0.298996746825692</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B184" s="6" t="n">
-        <v>0.00283375610792122</v>
+        <v>0.00283696814096522</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E184" s="0" t="n">
         <v>0</v>
@@ -4425,13 +4427,13 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>2.92237150620175</v>
+        <v>2.92139465665056</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E185" s="0" t="n">
         <v>100</v>
@@ -4442,30 +4444,30 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>2.45822499038235</v>
+        <v>2.45740328924902</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="E186" s="6" t="n">
-        <v>-1.04825308562963E-005</v>
+        <v>-1.10564882773044E-005</v>
       </c>
       <c r="G186" s="6" t="n">
-        <v>-1.0482E-005</v>
+        <v>-1.1056E-005</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>0.464146515819399</v>
+        <v>0.463991367401535</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E187" s="0" t="n">
         <v>0</v>
@@ -4473,36 +4475,37 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B188" s="6" t="n">
-        <v>5.23728843107264E-008</v>
+        <v>4.72790437531057E-008</v>
       </c>
       <c r="D188" s="0" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="E188" s="6" t="n">
-        <v>1.04121493855719E-005</v>
+        <v>1.09860270209717E-005</v>
       </c>
       <c r="G188" s="6" t="n">
-        <v>1.0411E-005</v>
+        <v>1.0985E-005</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B189" s="6" t="n">
-        <v>2.92197583899194E-005</v>
-      </c>
-      <c r="D189" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E189" s="6" t="n">
-        <v>1.41715691735777E-009</v>
-      </c>
-      <c r="G189" s="6" t="n">
-        <v>1.5189E-009</v>
+        <v>2.92197604047699E-005</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E189" s="8" t="n">
+        <v>1.40911384251758E-009</v>
+      </c>
+      <c r="F189" s="22"/>
+      <c r="G189" s="8" t="n">
+        <v>1.5116E-009</v>
       </c>
       <c r="I189" s="0" t="s">
         <v>88</v>
@@ -4510,39 +4513,42 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B190" s="6" t="n">
-        <v>2.1686620606511E-011</v>
+        <v>2.33807600936833E-011</v>
       </c>
       <c r="D190" s="7" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="E190" s="8" t="n">
-        <v>3.99681319740682E-009</v>
+        <v>3.72305921224692E-009</v>
       </c>
       <c r="F190" s="7"/>
       <c r="G190" s="8" t="n">
-        <v>-3.6624E-007</v>
+        <v>-3.6716E-007</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B191" s="6" t="n">
-        <v>3.09714372072542E-009</v>
+        <v>3.16426889455719E-009</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="E191" s="6" t="n">
-        <v>0.00662624658898784</v>
+        <v>0.00665011669805122</v>
+      </c>
+      <c r="G191" s="6" t="n">
+        <v>0.00665012</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B192" s="6" t="n">
         <v>7.3E-009</v>
@@ -4907,7 +4913,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="0"/>
@@ -4934,7 +4940,7 @@
       </c>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="24" t="s">
         <v>102</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -4942,7 +4948,7 @@
       </c>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
-      <c r="M8" s="23"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="9"/>
       <c r="S8" s="2" t="n">
         <f aca="false">IF(ABS(J8-F8)&lt;N$5,1,999)</f>
@@ -4964,7 +4970,7 @@
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="24" t="s">
         <v>107</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -4972,7 +4978,7 @@
       </c>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="24"/>
       <c r="N9" s="9"/>
       <c r="S9" s="2" t="n">
         <f aca="false">IF(ABS(J9-F9)&lt;N$5,1,999)</f>
@@ -4994,7 +5000,7 @@
       </c>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="24" t="s">
         <v>112</v>
       </c>
       <c r="J10" s="9" t="s">
@@ -5002,7 +5008,7 @@
       </c>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="9"/>
       <c r="S10" s="2" t="n">
         <f aca="false">IF(ABS(J10-F10)&lt;N$5,1,999)</f>
@@ -5024,7 +5030,7 @@
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="24" t="s">
         <v>115</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -5032,7 +5038,7 @@
       </c>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
-      <c r="M11" s="23"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="9"/>
       <c r="S11" s="2" t="n">
         <f aca="false">IF(ABS(J11-F11)&lt;N$5,1,999)</f>
@@ -5055,7 +5061,7 @@
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="24" t="s">
         <v>119</v>
       </c>
       <c r="J12" s="9" t="s">
@@ -5063,7 +5069,7 @@
       </c>
       <c r="K12" s="0"/>
       <c r="L12" s="0"/>
-      <c r="M12" s="23"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="9"/>
       <c r="S12" s="2" t="n">
         <f aca="false">IF(ABS(J12-F12)&lt;N$5,1,999)</f>
@@ -5086,7 +5092,7 @@
       </c>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="24" t="s">
         <v>123</v>
       </c>
       <c r="J13" s="9" t="s">
@@ -5094,7 +5100,7 @@
       </c>
       <c r="K13" s="0"/>
       <c r="L13" s="0"/>
-      <c r="M13" s="23"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="9"/>
       <c r="S13" s="2" t="n">
         <f aca="false">IF(ABS(J13-F13)&lt;N$5,1,999)</f>
@@ -5116,7 +5122,7 @@
       </c>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="24" t="s">
         <v>56</v>
       </c>
       <c r="J14" s="2" t="n">
@@ -5124,7 +5130,7 @@
       </c>
       <c r="K14" s="0"/>
       <c r="L14" s="0"/>
-      <c r="M14" s="23" t="s">
+      <c r="M14" s="24" t="s">
         <v>56</v>
       </c>
       <c r="N14" s="2" t="n">
@@ -5150,7 +5156,7 @@
       </c>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="24" t="s">
         <v>129</v>
       </c>
       <c r="J15" s="9" t="s">
@@ -5180,7 +5186,7 @@
       </c>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="9"/>
       <c r="K16" s="0"/>
       <c r="L16" s="0"/>
@@ -5202,7 +5208,7 @@
       </c>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="24" t="s">
         <v>134</v>
       </c>
       <c r="J17" s="9" t="s">
@@ -5232,7 +5238,7 @@
       </c>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="24" t="s">
         <v>139</v>
       </c>
       <c r="J18" s="6" t="n">
@@ -5262,7 +5268,7 @@
       </c>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="24" t="s">
         <v>142</v>
       </c>
       <c r="J19" s="6" t="n">
@@ -5270,7 +5276,7 @@
       </c>
       <c r="K19" s="0"/>
       <c r="L19" s="0"/>
-      <c r="M19" s="23" t="s">
+      <c r="M19" s="24" t="s">
         <v>58</v>
       </c>
       <c r="N19" s="6" t="n">
@@ -5296,7 +5302,7 @@
       </c>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="24" t="s">
         <v>59</v>
       </c>
       <c r="J20" s="9" t="s">
@@ -5304,7 +5310,7 @@
       </c>
       <c r="K20" s="0"/>
       <c r="L20" s="0"/>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="24" t="s">
         <v>59</v>
       </c>
       <c r="N20" s="2" t="n">
@@ -5330,7 +5336,7 @@
       </c>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="9"/>
       <c r="K21" s="0"/>
       <c r="L21" s="0"/>
@@ -5358,7 +5364,7 @@
       </c>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="24" t="s">
         <v>152</v>
       </c>
       <c r="J22" s="9" t="s">
@@ -5388,7 +5394,7 @@
       </c>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="24" t="s">
         <v>157</v>
       </c>
       <c r="J23" s="6" t="n">
@@ -5418,7 +5424,7 @@
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="24" t="s">
         <v>160</v>
       </c>
       <c r="J24" s="6" t="n">
@@ -5426,7 +5432,7 @@
       </c>
       <c r="K24" s="0"/>
       <c r="L24" s="0"/>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="24" t="s">
         <v>60</v>
       </c>
       <c r="N24" s="9" t="s">
@@ -5452,7 +5458,7 @@
       </c>
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
-      <c r="I25" s="23" t="s">
+      <c r="I25" s="24" t="s">
         <v>61</v>
       </c>
       <c r="J25" s="2" t="n">
@@ -5460,7 +5466,7 @@
       </c>
       <c r="K25" s="0"/>
       <c r="L25" s="0"/>
-      <c r="M25" s="23" t="s">
+      <c r="M25" s="24" t="s">
         <v>61</v>
       </c>
       <c r="N25" s="9" t="s">
@@ -5482,7 +5488,7 @@
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
-      <c r="I26" s="23"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="9"/>
       <c r="K26" s="0"/>
       <c r="L26" s="0"/>
@@ -5506,7 +5512,7 @@
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="23" t="s">
+      <c r="I27" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J27" s="9" t="s">
@@ -5532,7 +5538,7 @@
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="24" t="s">
         <v>168</v>
       </c>
       <c r="J28" s="9" t="s">
@@ -5558,7 +5564,7 @@
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="24" t="s">
         <v>173</v>
       </c>
       <c r="J29" s="6" t="n">
@@ -5566,7 +5572,7 @@
       </c>
       <c r="K29" s="0"/>
       <c r="L29" s="0"/>
-      <c r="M29" s="23" t="s">
+      <c r="M29" s="24" t="s">
         <v>62</v>
       </c>
       <c r="N29" s="9" t="s">
@@ -5588,7 +5594,7 @@
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="24" t="s">
         <v>175</v>
       </c>
       <c r="J30" s="9" t="s">
@@ -5596,7 +5602,7 @@
       </c>
       <c r="K30" s="0"/>
       <c r="L30" s="0"/>
-      <c r="M30" s="23" t="s">
+      <c r="M30" s="24" t="s">
         <v>63</v>
       </c>
       <c r="N30" s="6" t="n">
@@ -5618,7 +5624,7 @@
       </c>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
-      <c r="I31" s="23"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
       <c r="L31" s="0"/>
@@ -5642,7 +5648,7 @@
       </c>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="24" t="s">
         <v>179</v>
       </c>
       <c r="J32" s="6" t="n">
@@ -5650,7 +5656,7 @@
       </c>
       <c r="K32" s="0"/>
       <c r="L32" s="0"/>
-      <c r="M32" s="23" t="s">
+      <c r="M32" s="24" t="s">
         <v>64</v>
       </c>
       <c r="N32" s="6" t="n">
@@ -5672,7 +5678,7 @@
       </c>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
-      <c r="I33" s="23"/>
+      <c r="I33" s="24"/>
       <c r="J33" s="6"/>
       <c r="K33" s="0"/>
       <c r="L33" s="0"/>
@@ -5704,7 +5710,7 @@
       </c>
       <c r="K34" s="0"/>
       <c r="L34" s="0"/>
-      <c r="M34" s="23" t="s">
+      <c r="M34" s="24" t="s">
         <v>65</v>
       </c>
       <c r="N34" s="9" t="s">
@@ -5734,7 +5740,7 @@
       </c>
       <c r="K35" s="0"/>
       <c r="L35" s="0"/>
-      <c r="M35" s="23" t="s">
+      <c r="M35" s="24" t="s">
         <v>66</v>
       </c>
       <c r="N35" s="9" t="s">
@@ -5763,7 +5769,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="0"/>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="24" t="s">
         <v>188</v>
       </c>
       <c r="F37" s="2" t="n">
@@ -5771,7 +5777,7 @@
       </c>
       <c r="G37" s="0"/>
       <c r="H37" s="0"/>
-      <c r="I37" s="23" t="s">
+      <c r="I37" s="24" t="s">
         <v>189</v>
       </c>
       <c r="J37" s="2" t="n">
@@ -5779,7 +5785,7 @@
       </c>
       <c r="K37" s="0"/>
       <c r="L37" s="0"/>
-      <c r="M37" s="23" t="s">
+      <c r="M37" s="24" t="s">
         <v>67</v>
       </c>
       <c r="N37" s="9" t="s">
@@ -5790,30 +5796,30 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
       <c r="B38" s="0"/>
-      <c r="E38" s="23"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="0"/>
       <c r="G38" s="0"/>
       <c r="H38" s="0"/>
-      <c r="I38" s="23"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="0"/>
       <c r="K38" s="0"/>
       <c r="L38" s="0"/>
-      <c r="M38" s="23"/>
+      <c r="M38" s="24"/>
       <c r="N38" s="9"/>
       <c r="S38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
       <c r="B39" s="0"/>
-      <c r="E39" s="23"/>
+      <c r="E39" s="24"/>
       <c r="F39" s="0"/>
       <c r="G39" s="0"/>
       <c r="H39" s="0"/>
-      <c r="I39" s="23"/>
+      <c r="I39" s="24"/>
       <c r="J39" s="0"/>
       <c r="K39" s="0"/>
       <c r="L39" s="0"/>
-      <c r="M39" s="23"/>
+      <c r="M39" s="24"/>
       <c r="N39" s="9"/>
       <c r="S39" s="0"/>
     </row>
@@ -6625,7 +6631,7 @@
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
       <c r="B70" s="0"/>
-      <c r="E70" s="23" t="s">
+      <c r="E70" s="24" t="s">
         <v>188</v>
       </c>
       <c r="F70" s="2" t="n">
@@ -6636,7 +6642,7 @@
       <c r="I70" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="J70" s="23" t="n">
+      <c r="J70" s="24" t="n">
         <v>0.487643152</v>
       </c>
       <c r="M70" s="2" t="s">
@@ -7018,7 +7024,7 @@
       <c r="A88" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B88" s="25" t="s">
         <v>197</v>
       </c>
       <c r="E88" s="2" t="s">
@@ -7038,7 +7044,7 @@
       <c r="A89" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B89" s="25" t="s">
         <v>148</v>
       </c>
       <c r="E89" s="2" t="s">
@@ -7062,7 +7068,7 @@
       <c r="A90" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B90" s="24" t="s">
+      <c r="B90" s="25" t="s">
         <v>151</v>
       </c>
       <c r="E90" s="2" t="s">
@@ -7086,7 +7092,7 @@
       <c r="A91" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" s="25" t="s">
         <v>156</v>
       </c>
       <c r="E91" s="2" t="s">
@@ -7365,7 +7371,7 @@
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
       <c r="B104" s="0"/>
-      <c r="E104" s="23" t="s">
+      <c r="E104" s="24" t="s">
         <v>188</v>
       </c>
       <c r="F104" s="2" t="n">
@@ -7374,7 +7380,7 @@
       <c r="G104" s="0"/>
       <c r="H104" s="0"/>
       <c r="I104" s="0"/>
-      <c r="J104" s="25" t="n">
+      <c r="J104" s="26" t="n">
         <v>0.0277557671</v>
       </c>
       <c r="M104" s="2" t="s">
@@ -7550,7 +7556,7 @@
       <c r="A114" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B114" s="26" t="n">
+      <c r="B114" s="27" t="n">
         <v>0.1</v>
       </c>
       <c r="E114" s="2" t="s">
@@ -7574,7 +7580,7 @@
       <c r="A115" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B115" s="26" t="n">
+      <c r="B115" s="27" t="n">
         <v>1</v>
       </c>
       <c r="E115" s="2" t="s">
@@ -7607,12 +7613,12 @@
       <c r="F116" s="2" t="n">
         <v>49.5121</v>
       </c>
-      <c r="G116" s="27"/>
-      <c r="H116" s="27"/>
-      <c r="I116" s="27" t="s">
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J116" s="27" t="n">
+      <c r="J116" s="7" t="n">
         <v>49.5110397</v>
       </c>
       <c r="M116" s="2" t="s">
@@ -7742,7 +7748,7 @@
       <c r="A122" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B122" s="24" t="s">
+      <c r="B122" s="25" t="s">
         <v>201</v>
       </c>
       <c r="E122" s="2" t="s">
@@ -7751,18 +7757,18 @@
       <c r="F122" s="2" t="n">
         <v>59.9192</v>
       </c>
-      <c r="G122" s="27"/>
-      <c r="H122" s="27"/>
-      <c r="I122" s="27" t="s">
+      <c r="G122" s="7"/>
+      <c r="H122" s="7"/>
+      <c r="I122" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="J122" s="27" t="n">
+      <c r="J122" s="7" t="n">
         <v>59.9179878</v>
       </c>
       <c r="M122" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N122" s="27" t="n">
+      <c r="N122" s="7" t="n">
         <v>59.9191652451627</v>
       </c>
     </row>
@@ -7770,7 +7776,7 @@
       <c r="A123" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B123" s="24" t="s">
+      <c r="B123" s="25" t="s">
         <v>202</v>
       </c>
       <c r="E123" s="2" t="s">
@@ -7788,7 +7794,7 @@
       <c r="A124" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B124" s="24" t="s">
+      <c r="B124" s="25" t="s">
         <v>151</v>
       </c>
       <c r="E124" s="2" t="s">
@@ -7810,7 +7816,7 @@
       <c r="A125" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B125" s="24" t="s">
+      <c r="B125" s="25" t="s">
         <v>156</v>
       </c>
       <c r="E125" s="2" t="s">
@@ -8057,7 +8063,7 @@
       <c r="N138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E139" s="23" t="s">
+      <c r="E139" s="24" t="s">
         <v>188</v>
       </c>
       <c r="F139" s="2" t="n">
@@ -8216,7 +8222,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="0"/>
@@ -8242,7 +8248,7 @@
       </c>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="24" t="s">
         <v>102</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -8271,7 +8277,7 @@
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="24" t="s">
         <v>107</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -8300,7 +8306,7 @@
       </c>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="24" t="s">
         <v>112</v>
       </c>
       <c r="J10" s="9" t="s">
@@ -8329,7 +8335,7 @@
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="24" t="s">
         <v>115</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -8359,7 +8365,7 @@
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="24" t="s">
         <v>119</v>
       </c>
       <c r="J12" s="9" t="s">
@@ -8389,7 +8395,7 @@
       </c>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="24" t="s">
         <v>123</v>
       </c>
       <c r="J13" s="9" t="s">
@@ -8418,7 +8424,7 @@
       </c>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="24" t="s">
         <v>56</v>
       </c>
       <c r="J14" s="2" t="n">
@@ -8447,7 +8453,7 @@
       </c>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="24" t="s">
         <v>129</v>
       </c>
       <c r="J15" s="2" t="n">
@@ -8476,7 +8482,7 @@
       </c>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
       <c r="L16" s="0"/>
@@ -8499,7 +8505,7 @@
       </c>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="24" t="s">
         <v>134</v>
       </c>
       <c r="J17" s="9" t="s">
@@ -8528,7 +8534,7 @@
       </c>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="24" t="s">
         <v>139</v>
       </c>
       <c r="J18" s="9" t="s">
@@ -8557,7 +8563,7 @@
       </c>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="24" t="s">
         <v>142</v>
       </c>
       <c r="J19" s="9" t="s">
@@ -8586,7 +8592,7 @@
       </c>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="24" t="s">
         <v>59</v>
       </c>
       <c r="J20" s="2" t="n">
@@ -8615,7 +8621,7 @@
       </c>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
       <c r="L21" s="0"/>
@@ -8642,7 +8648,7 @@
       </c>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="24" t="s">
         <v>152</v>
       </c>
       <c r="J22" s="9" t="s">
@@ -8671,7 +8677,7 @@
       </c>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="24" t="s">
         <v>157</v>
       </c>
       <c r="J23" s="9" t="s">
@@ -8700,7 +8706,7 @@
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="24" t="s">
         <v>160</v>
       </c>
       <c r="J24" s="9" t="s">
@@ -8729,7 +8735,7 @@
       </c>
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
-      <c r="I25" s="23" t="s">
+      <c r="I25" s="24" t="s">
         <v>61</v>
       </c>
       <c r="J25" s="2" t="n">
@@ -8754,7 +8760,7 @@
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
-      <c r="I26" s="23"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
       <c r="L26" s="0"/>
@@ -8777,7 +8783,7 @@
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="23" t="s">
+      <c r="I27" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J27" s="2" t="n">
@@ -8802,7 +8808,7 @@
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="24" t="s">
         <v>168</v>
       </c>
       <c r="J28" s="9" t="s">
@@ -8827,7 +8833,7 @@
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="24" t="s">
         <v>173</v>
       </c>
       <c r="J29" s="9" t="s">
@@ -8852,7 +8858,7 @@
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="24" t="s">
         <v>175</v>
       </c>
       <c r="J30" s="9" t="s">
@@ -8877,7 +8883,7 @@
       </c>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
-      <c r="I31" s="23"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
       <c r="L31" s="0"/>
@@ -8900,7 +8906,7 @@
       </c>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="24" t="s">
         <v>179</v>
       </c>
       <c r="J32" s="9" t="s">
@@ -8925,7 +8931,7 @@
       </c>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
-      <c r="I33" s="23"/>
+      <c r="I33" s="24"/>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
       <c r="L33" s="0"/>
@@ -8948,7 +8954,7 @@
       </c>
       <c r="G34" s="0"/>
       <c r="H34" s="0"/>
-      <c r="I34" s="23" t="s">
+      <c r="I34" s="24" t="s">
         <v>183</v>
       </c>
       <c r="J34" s="6" t="n">
@@ -8973,7 +8979,7 @@
       </c>
       <c r="G35" s="0"/>
       <c r="H35" s="0"/>
-      <c r="I35" s="23" t="s">
+      <c r="I35" s="24" t="s">
         <v>186</v>
       </c>
       <c r="J35" s="6" t="n">
@@ -17553,7 +17559,7 @@
       <c r="A392" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B392" s="24" t="s">
+      <c r="B392" s="25" t="s">
         <v>197</v>
       </c>
       <c r="E392" s="28" t="s">
@@ -17582,7 +17588,7 @@
       <c r="A393" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B393" s="24" t="s">
+      <c r="B393" s="25" t="s">
         <v>148</v>
       </c>
       <c r="E393" s="2" t="s">
@@ -17609,7 +17615,7 @@
       <c r="A394" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B394" s="24" t="s">
+      <c r="B394" s="25" t="s">
         <v>151</v>
       </c>
       <c r="E394" s="2" t="s">
@@ -17638,7 +17644,7 @@
       <c r="A395" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B395" s="24" t="s">
+      <c r="B395" s="25" t="s">
         <v>156</v>
       </c>
       <c r="E395" s="2" t="s">
@@ -18141,7 +18147,7 @@
       <c r="A416" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B416" s="26" t="n">
+      <c r="B416" s="27" t="n">
         <v>0.1</v>
       </c>
       <c r="E416" s="28" t="s">
@@ -18170,7 +18176,7 @@
       <c r="A417" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B417" s="26" t="n">
+      <c r="B417" s="27" t="n">
         <v>1</v>
       </c>
       <c r="E417" s="28" t="s">
@@ -18367,7 +18373,7 @@
       <c r="A424" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B424" s="24" t="s">
+      <c r="B424" s="25" t="s">
         <v>201</v>
       </c>
       <c r="E424" s="28" t="s">
@@ -18396,7 +18402,7 @@
       <c r="A425" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B425" s="24" t="s">
+      <c r="B425" s="25" t="s">
         <v>202</v>
       </c>
       <c r="E425" s="2" t="s">
@@ -18423,7 +18429,7 @@
       <c r="A426" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B426" s="24" t="s">
+      <c r="B426" s="25" t="s">
         <v>151</v>
       </c>
       <c r="E426" s="2" t="s">
@@ -18452,7 +18458,7 @@
       <c r="A427" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B427" s="24" t="s">
+      <c r="B427" s="25" t="s">
         <v>156</v>
       </c>
       <c r="E427" s="2" t="s">
@@ -18899,7 +18905,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>244</v>
       </c>
       <c r="B8" s="0"/>
@@ -19100,7 +19106,7 @@
       </c>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="24" t="s">
         <v>129</v>
       </c>
       <c r="J16" s="2" t="n">
@@ -19125,7 +19131,7 @@
       </c>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
       <c r="L17" s="0"/>
@@ -19148,7 +19154,7 @@
       </c>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="24" t="s">
         <v>134</v>
       </c>
       <c r="J18" s="9" t="s">
@@ -19173,7 +19179,7 @@
       </c>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="24" t="s">
         <v>139</v>
       </c>
       <c r="J19" s="9" t="s">
@@ -19248,7 +19254,7 @@
       </c>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
       <c r="L22" s="0"/>
@@ -19271,7 +19277,7 @@
       </c>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="24" t="s">
         <v>152</v>
       </c>
       <c r="J23" s="9" t="s">
@@ -19296,7 +19302,7 @@
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="24" t="s">
         <v>157</v>
       </c>
       <c r="J24" s="9" t="s">
@@ -19371,7 +19377,7 @@
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="23"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
       <c r="L27" s="0"/>
@@ -19394,7 +19400,7 @@
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J28" s="2" t="n">
@@ -19419,7 +19425,7 @@
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="24" t="s">
         <v>168</v>
       </c>
       <c r="J29" s="9" t="s">
@@ -19494,7 +19500,7 @@
       </c>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
-      <c r="I32" s="23"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
       <c r="L32" s="0"/>
@@ -19542,7 +19548,7 @@
       </c>
       <c r="G34" s="0"/>
       <c r="H34" s="0"/>
-      <c r="I34" s="23"/>
+      <c r="I34" s="24"/>
       <c r="J34" s="0"/>
       <c r="K34" s="0"/>
       <c r="L34" s="0"/>
@@ -19655,7 +19661,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="23" t="s">
         <v>275</v>
       </c>
       <c r="B40" s="0"/>
@@ -19856,7 +19862,7 @@
       </c>
       <c r="G48" s="0"/>
       <c r="H48" s="0"/>
-      <c r="I48" s="23" t="s">
+      <c r="I48" s="24" t="s">
         <v>129</v>
       </c>
       <c r="J48" s="2" t="n">
@@ -19881,7 +19887,7 @@
       </c>
       <c r="G49" s="0"/>
       <c r="H49" s="0"/>
-      <c r="I49" s="23"/>
+      <c r="I49" s="24"/>
       <c r="J49" s="0"/>
       <c r="K49" s="0"/>
       <c r="L49" s="0"/>
@@ -19904,7 +19910,7 @@
       </c>
       <c r="G50" s="0"/>
       <c r="H50" s="0"/>
-      <c r="I50" s="23" t="s">
+      <c r="I50" s="24" t="s">
         <v>134</v>
       </c>
       <c r="J50" s="9" t="s">
@@ -19929,7 +19935,7 @@
       </c>
       <c r="G51" s="0"/>
       <c r="H51" s="0"/>
-      <c r="I51" s="23" t="s">
+      <c r="I51" s="24" t="s">
         <v>139</v>
       </c>
       <c r="J51" s="9" t="s">
@@ -20004,7 +20010,7 @@
       </c>
       <c r="G54" s="0"/>
       <c r="H54" s="0"/>
-      <c r="I54" s="23"/>
+      <c r="I54" s="24"/>
       <c r="J54" s="0"/>
       <c r="K54" s="0"/>
       <c r="L54" s="0"/>
@@ -20027,7 +20033,7 @@
       </c>
       <c r="G55" s="0"/>
       <c r="H55" s="0"/>
-      <c r="I55" s="23" t="s">
+      <c r="I55" s="24" t="s">
         <v>152</v>
       </c>
       <c r="J55" s="9" t="s">
@@ -20052,7 +20058,7 @@
       </c>
       <c r="G56" s="0"/>
       <c r="H56" s="0"/>
-      <c r="I56" s="23" t="s">
+      <c r="I56" s="24" t="s">
         <v>157</v>
       </c>
       <c r="J56" s="9" t="s">
@@ -20127,7 +20133,7 @@
       </c>
       <c r="G59" s="0"/>
       <c r="H59" s="0"/>
-      <c r="I59" s="23"/>
+      <c r="I59" s="24"/>
       <c r="J59" s="0"/>
       <c r="K59" s="0"/>
       <c r="L59" s="0"/>
@@ -20150,7 +20156,7 @@
       </c>
       <c r="G60" s="0"/>
       <c r="H60" s="0"/>
-      <c r="I60" s="23" t="s">
+      <c r="I60" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J60" s="2" t="n">
@@ -20175,7 +20181,7 @@
       </c>
       <c r="G61" s="0"/>
       <c r="H61" s="0"/>
-      <c r="I61" s="23" t="s">
+      <c r="I61" s="24" t="s">
         <v>168</v>
       </c>
       <c r="J61" s="9" t="s">
@@ -20250,7 +20256,7 @@
       </c>
       <c r="G64" s="0"/>
       <c r="H64" s="0"/>
-      <c r="I64" s="23"/>
+      <c r="I64" s="24"/>
       <c r="J64" s="0"/>
       <c r="K64" s="0"/>
       <c r="L64" s="0"/>
@@ -20298,7 +20304,7 @@
       </c>
       <c r="G66" s="0"/>
       <c r="H66" s="0"/>
-      <c r="I66" s="23"/>
+      <c r="I66" s="24"/>
       <c r="J66" s="0"/>
       <c r="K66" s="0"/>
       <c r="L66" s="0"/>
@@ -20411,7 +20417,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="23" t="s">
         <v>307</v>
       </c>
       <c r="B72" s="0"/>
@@ -20612,7 +20618,7 @@
       </c>
       <c r="G80" s="0"/>
       <c r="H80" s="0"/>
-      <c r="I80" s="23" t="s">
+      <c r="I80" s="24" t="s">
         <v>129</v>
       </c>
       <c r="J80" s="2" t="n">
@@ -20637,7 +20643,7 @@
       </c>
       <c r="G81" s="0"/>
       <c r="H81" s="0"/>
-      <c r="I81" s="23"/>
+      <c r="I81" s="24"/>
       <c r="J81" s="0"/>
       <c r="K81" s="0"/>
       <c r="L81" s="0"/>
@@ -20660,7 +20666,7 @@
       </c>
       <c r="G82" s="0"/>
       <c r="H82" s="0"/>
-      <c r="I82" s="23" t="s">
+      <c r="I82" s="24" t="s">
         <v>134</v>
       </c>
       <c r="J82" s="9" t="s">
@@ -20685,7 +20691,7 @@
       </c>
       <c r="G83" s="0"/>
       <c r="H83" s="0"/>
-      <c r="I83" s="23" t="s">
+      <c r="I83" s="24" t="s">
         <v>139</v>
       </c>
       <c r="J83" s="9" t="s">
@@ -20760,7 +20766,7 @@
       </c>
       <c r="G86" s="0"/>
       <c r="H86" s="0"/>
-      <c r="I86" s="23"/>
+      <c r="I86" s="24"/>
       <c r="J86" s="0"/>
       <c r="K86" s="0"/>
       <c r="L86" s="0"/>
@@ -20783,7 +20789,7 @@
       </c>
       <c r="G87" s="0"/>
       <c r="H87" s="0"/>
-      <c r="I87" s="23" t="s">
+      <c r="I87" s="24" t="s">
         <v>152</v>
       </c>
       <c r="J87" s="9" t="s">
@@ -20808,7 +20814,7 @@
       </c>
       <c r="G88" s="0"/>
       <c r="H88" s="0"/>
-      <c r="I88" s="23" t="s">
+      <c r="I88" s="24" t="s">
         <v>157</v>
       </c>
       <c r="J88" s="9" t="s">
@@ -20883,7 +20889,7 @@
       </c>
       <c r="G91" s="0"/>
       <c r="H91" s="0"/>
-      <c r="I91" s="23"/>
+      <c r="I91" s="24"/>
       <c r="J91" s="0"/>
       <c r="K91" s="0"/>
       <c r="L91" s="0"/>
@@ -20906,7 +20912,7 @@
       </c>
       <c r="G92" s="0"/>
       <c r="H92" s="0"/>
-      <c r="I92" s="23" t="s">
+      <c r="I92" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J92" s="2" t="n">
@@ -20931,7 +20937,7 @@
       </c>
       <c r="G93" s="0"/>
       <c r="H93" s="0"/>
-      <c r="I93" s="23" t="s">
+      <c r="I93" s="24" t="s">
         <v>168</v>
       </c>
       <c r="J93" s="9" t="s">
@@ -21006,7 +21012,7 @@
       </c>
       <c r="G96" s="0"/>
       <c r="H96" s="0"/>
-      <c r="I96" s="23"/>
+      <c r="I96" s="24"/>
       <c r="J96" s="0"/>
       <c r="K96" s="0"/>
       <c r="L96" s="0"/>
@@ -21054,7 +21060,7 @@
       </c>
       <c r="G98" s="0"/>
       <c r="H98" s="0"/>
-      <c r="I98" s="23"/>
+      <c r="I98" s="24"/>
       <c r="J98" s="0"/>
       <c r="K98" s="0"/>
       <c r="L98" s="0"/>
@@ -21167,7 +21173,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="22" t="s">
+      <c r="A104" s="23" t="s">
         <v>339</v>
       </c>
       <c r="B104" s="0"/>
@@ -21344,7 +21350,7 @@
       </c>
       <c r="G112" s="0"/>
       <c r="H112" s="0"/>
-      <c r="I112" s="23"/>
+      <c r="I112" s="24"/>
       <c r="J112" s="0"/>
       <c r="K112" s="0"/>
       <c r="L112" s="0"/>
@@ -21365,7 +21371,7 @@
       </c>
       <c r="G113" s="0"/>
       <c r="H113" s="0"/>
-      <c r="I113" s="23"/>
+      <c r="I113" s="24"/>
       <c r="J113" s="0"/>
       <c r="K113" s="0"/>
       <c r="L113" s="0"/>
@@ -21388,7 +21394,7 @@
       </c>
       <c r="G114" s="0"/>
       <c r="H114" s="0"/>
-      <c r="I114" s="23"/>
+      <c r="I114" s="24"/>
       <c r="J114" s="9"/>
       <c r="K114" s="0"/>
       <c r="L114" s="0"/>
@@ -21409,7 +21415,7 @@
       </c>
       <c r="G115" s="0"/>
       <c r="H115" s="0"/>
-      <c r="I115" s="23"/>
+      <c r="I115" s="24"/>
       <c r="J115" s="9"/>
       <c r="K115" s="0"/>
       <c r="L115" s="0"/>
@@ -21472,7 +21478,7 @@
       </c>
       <c r="G118" s="0"/>
       <c r="H118" s="0"/>
-      <c r="I118" s="23"/>
+      <c r="I118" s="24"/>
       <c r="J118" s="0"/>
       <c r="K118" s="0"/>
       <c r="L118" s="0"/>
@@ -21495,7 +21501,7 @@
       </c>
       <c r="G119" s="0"/>
       <c r="H119" s="0"/>
-      <c r="I119" s="23"/>
+      <c r="I119" s="24"/>
       <c r="J119" s="9"/>
       <c r="K119" s="0"/>
       <c r="L119" s="0"/>
@@ -21516,7 +21522,7 @@
       </c>
       <c r="G120" s="0"/>
       <c r="H120" s="0"/>
-      <c r="I120" s="23"/>
+      <c r="I120" s="24"/>
       <c r="J120" s="9"/>
       <c r="K120" s="0"/>
       <c r="L120" s="0"/>
@@ -21579,7 +21585,7 @@
       </c>
       <c r="G123" s="0"/>
       <c r="H123" s="0"/>
-      <c r="I123" s="23"/>
+      <c r="I123" s="24"/>
       <c r="J123" s="0"/>
       <c r="K123" s="0"/>
       <c r="L123" s="0"/>
@@ -21602,7 +21608,7 @@
       </c>
       <c r="G124" s="0"/>
       <c r="H124" s="0"/>
-      <c r="I124" s="23"/>
+      <c r="I124" s="24"/>
       <c r="J124" s="0"/>
       <c r="K124" s="0"/>
       <c r="L124" s="0"/>
@@ -21623,7 +21629,7 @@
       </c>
       <c r="G125" s="0"/>
       <c r="H125" s="0"/>
-      <c r="I125" s="23"/>
+      <c r="I125" s="24"/>
       <c r="J125" s="9"/>
       <c r="K125" s="0"/>
       <c r="L125" s="0"/>
@@ -21686,7 +21692,7 @@
       </c>
       <c r="G128" s="0"/>
       <c r="H128" s="0"/>
-      <c r="I128" s="23"/>
+      <c r="I128" s="24"/>
       <c r="J128" s="0"/>
       <c r="K128" s="0"/>
       <c r="L128" s="0"/>
@@ -21730,7 +21736,7 @@
       </c>
       <c r="G130" s="0"/>
       <c r="H130" s="0"/>
-      <c r="I130" s="23"/>
+      <c r="I130" s="24"/>
       <c r="J130" s="0"/>
       <c r="K130" s="0"/>
       <c r="L130" s="0"/>
@@ -21835,7 +21841,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="22" t="s">
+      <c r="A136" s="23" t="s">
         <v>339</v>
       </c>
       <c r="B136" s="0"/>
@@ -22036,7 +22042,7 @@
       </c>
       <c r="G144" s="0"/>
       <c r="H144" s="0"/>
-      <c r="I144" s="23" t="s">
+      <c r="I144" s="24" t="s">
         <v>129</v>
       </c>
       <c r="J144" s="2" t="n">
@@ -22060,7 +22066,7 @@
       </c>
       <c r="G145" s="0"/>
       <c r="H145" s="0"/>
-      <c r="I145" s="23"/>
+      <c r="I145" s="24"/>
       <c r="J145" s="0"/>
       <c r="K145" s="0"/>
       <c r="L145" s="0"/>
@@ -22082,7 +22088,7 @@
       </c>
       <c r="G146" s="0"/>
       <c r="H146" s="0"/>
-      <c r="I146" s="23" t="s">
+      <c r="I146" s="24" t="s">
         <v>134</v>
       </c>
       <c r="J146" s="9" t="s">
@@ -22106,7 +22112,7 @@
       </c>
       <c r="G147" s="0"/>
       <c r="H147" s="0"/>
-      <c r="I147" s="23" t="s">
+      <c r="I147" s="24" t="s">
         <v>139</v>
       </c>
       <c r="J147" s="9" t="s">
@@ -22178,7 +22184,7 @@
       </c>
       <c r="G150" s="0"/>
       <c r="H150" s="0"/>
-      <c r="I150" s="23"/>
+      <c r="I150" s="24"/>
       <c r="J150" s="0"/>
       <c r="K150" s="0"/>
       <c r="L150" s="0"/>
@@ -22200,7 +22206,7 @@
       </c>
       <c r="G151" s="0"/>
       <c r="H151" s="0"/>
-      <c r="I151" s="23" t="s">
+      <c r="I151" s="24" t="s">
         <v>152</v>
       </c>
       <c r="J151" s="9" t="s">
@@ -22224,7 +22230,7 @@
       </c>
       <c r="G152" s="0"/>
       <c r="H152" s="0"/>
-      <c r="I152" s="23" t="s">
+      <c r="I152" s="24" t="s">
         <v>157</v>
       </c>
       <c r="J152" s="9" t="s">
@@ -22295,7 +22301,7 @@
       </c>
       <c r="G155" s="0"/>
       <c r="H155" s="0"/>
-      <c r="I155" s="23"/>
+      <c r="I155" s="24"/>
       <c r="J155" s="0"/>
       <c r="K155" s="0"/>
       <c r="L155" s="0"/>
@@ -22316,7 +22322,7 @@
       </c>
       <c r="G156" s="0"/>
       <c r="H156" s="0"/>
-      <c r="I156" s="23" t="s">
+      <c r="I156" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J156" s="2" t="n">
@@ -22339,7 +22345,7 @@
       </c>
       <c r="G157" s="0"/>
       <c r="H157" s="0"/>
-      <c r="I157" s="23" t="s">
+      <c r="I157" s="24" t="s">
         <v>168</v>
       </c>
       <c r="J157" s="9" t="s">
@@ -22408,7 +22414,7 @@
       </c>
       <c r="G160" s="0"/>
       <c r="H160" s="0"/>
-      <c r="I160" s="23"/>
+      <c r="I160" s="24"/>
       <c r="J160" s="0"/>
       <c r="K160" s="0"/>
       <c r="L160" s="0"/>
@@ -22452,7 +22458,7 @@
       </c>
       <c r="G162" s="0"/>
       <c r="H162" s="0"/>
-      <c r="I162" s="23"/>
+      <c r="I162" s="24"/>
       <c r="J162" s="0"/>
       <c r="K162" s="0"/>
       <c r="L162" s="0"/>

</xml_diff>